<commit_message>
added attendence and fees page
</commit_message>
<xml_diff>
--- a/public/uploads/AIDS_A.xlsx
+++ b/public/uploads/AIDS_A.xlsx
@@ -2,39 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aabccfe195a227aa/Desktop/Mini Project/student-management/uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fcf122ec968ba018/Documents/Krish/VS Code/Mini-Project/public/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BE9949B-14DC-4F8C-AF24-4B9EFDE1D222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_5E43C013471C9F25E3116C3054E481A1BDF07F93" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE18ED99-BA7E-40E3-94ED-EDFA5A719E4D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8233A3AE-8D3C-4A27-AE86-BB09FB2FAF6E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="A" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -52,6 +38,21 @@
   </si>
   <si>
     <t>degree</t>
+  </si>
+  <si>
+    <t>Krish</t>
+  </si>
+  <si>
+    <t>vu4f2324074@pvppcoe.ac.in</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>aids</t>
   </si>
 </sst>
 </file>
@@ -60,7 +61,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -94,7 +95,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -402,16 +403,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37D0416-E893-4CB2-ADCF-F3C9ED34DA69}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,9 +428,32 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>